<commit_message>
Billing request report with datetime format
</commit_message>
<xml_diff>
--- a/reports/billing_requests/template.xlsx
+++ b/reports/billing_requests/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/cnctcli/reports/connect-reports/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/cnctcli/reports/connect-reports/reports/billing_requests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D43A12-18CB-EF4A-B3E6-AF7271975520}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7E70FC-FEBE-2341-877A-A2229935DC73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36760" yWindow="500" windowWidth="35840" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,15 +457,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="3" customWidth="1"/>
+    <col min="2" max="3" width="18.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
@@ -493,7 +492,7 @@
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="2" t="s">

</xml_diff>

<commit_message>
Added description to parameters, updated templates and unified way to pass data
</commit_message>
<xml_diff>
--- a/reports/billing_requests/template.xlsx
+++ b/reports/billing_requests/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/cnctcli/reports/connect-reports/reports/billing_requests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7E70FC-FEBE-2341-877A-A2229935DC73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF568487-BDCE-BE4C-9B48-846F1D64CF31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36760" yWindow="500" windowWidth="35840" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AB$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AH$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Item Name</t>
   </si>
@@ -52,18 +52,6 @@
     <t>Customer External ID</t>
   </si>
   <si>
-    <t>Provider Account ID</t>
-  </si>
-  <si>
-    <t>Provider Account name</t>
-  </si>
-  <si>
-    <t>Vendor Account ID</t>
-  </si>
-  <si>
-    <t>Vendor Account Name</t>
-  </si>
-  <si>
     <t>Product ID</t>
   </si>
   <si>
@@ -107,6 +95,36 @@
   </si>
   <si>
     <t>Subscription Type</t>
+  </si>
+  <si>
+    <t>Tier 1 ID</t>
+  </si>
+  <si>
+    <t>Tier 1 Name</t>
+  </si>
+  <si>
+    <t>Tier 1 Exrternal ID</t>
+  </si>
+  <si>
+    <t>Tier 2 ID</t>
+  </si>
+  <si>
+    <t>Tier 2 Name</t>
+  </si>
+  <si>
+    <t>Tier 2 Exrternal ID</t>
+  </si>
+  <si>
+    <t>Vendor ID</t>
+  </si>
+  <si>
+    <t>Provider ID</t>
+  </si>
+  <si>
+    <t>Provider Name</t>
+  </si>
+  <si>
+    <t>Vendor  Name</t>
   </si>
 </sst>
 </file>
@@ -455,60 +473,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="3" width="18.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="18.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="20" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="45.83203125" customWidth="1"/>
-    <col min="9" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="45.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="10" width="15" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="45.83203125" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
-    <col min="15" max="15" width="45.83203125" customWidth="1"/>
-    <col min="16" max="17" width="20" customWidth="1"/>
-    <col min="18" max="18" width="45.83203125" customWidth="1"/>
-    <col min="19" max="19" width="15" customWidth="1"/>
-    <col min="20" max="20" width="45.83203125" customWidth="1"/>
-    <col min="21" max="21" width="20" customWidth="1"/>
-    <col min="22" max="22" width="45.83203125" customWidth="1"/>
-    <col min="23" max="23" width="25.83203125" customWidth="1"/>
-    <col min="24" max="26" width="20" customWidth="1"/>
-    <col min="27" max="27" width="15" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="20" customWidth="1"/>
+    <col min="23" max="23" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="45.83203125" customWidth="1"/>
+    <col min="25" max="25" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="45.83203125" customWidth="1"/>
+    <col min="27" max="27" width="20" customWidth="1" outlineLevel="1"/>
     <col min="28" max="28" width="45.83203125" customWidth="1"/>
+    <col min="29" max="29" width="25.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="31" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="20" customWidth="1"/>
+    <col min="33" max="33" width="15" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -538,44 +565,62 @@
         <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
+  <autoFilter ref="A1:AH1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added per line item and not line item FF and Billing reports
</commit_message>
<xml_diff>
--- a/reports/billing_requests/template.xlsx
+++ b/reports/billing_requests/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/cnctcli/reports/connect-reports/reports/billing_requests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF568487-BDCE-BE4C-9B48-846F1D64CF31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A819FC-36A1-BC4E-B727-3C87DB5556AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36760" yWindow="500" windowWidth="35840" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,32 +16,14 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AH$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$Z$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
-  <si>
-    <t>Item Name</t>
-  </si>
-  <si>
-    <t>Item Type</t>
-  </si>
-  <si>
-    <t>Item Unit Of measure</t>
-  </si>
-  <si>
-    <t>Item MPN</t>
-  </si>
-  <si>
-    <t>Item Period</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Customer ID</t>
   </si>
@@ -77,12 +59,6 @@
   </si>
   <si>
     <t>Uom</t>
-  </si>
-  <si>
-    <t>Billing Cycle</t>
-  </si>
-  <si>
-    <t>Item Id</t>
   </si>
   <si>
     <t>Subscription ID</t>
@@ -473,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AH1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -484,143 +460,112 @@
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" style="3" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="18.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="10" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="20" customWidth="1"/>
-    <col min="23" max="23" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="45.83203125" customWidth="1"/>
-    <col min="25" max="25" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="10.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="45.83203125" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="45.83203125" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="45.83203125" customWidth="1"/>
+    <col min="21" max="21" width="25.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="23" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="20" customWidth="1"/>
+    <col min="25" max="25" width="15" customWidth="1" outlineLevel="1"/>
     <col min="26" max="26" width="45.83203125" customWidth="1"/>
-    <col min="27" max="27" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="45.83203125" customWidth="1"/>
-    <col min="29" max="29" width="25.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="31" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="20" customWidth="1"/>
-    <col min="33" max="33" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
+  <autoFilter ref="A1:Z1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>